<commit_message>
I think I understand the Alts
</commit_message>
<xml_diff>
--- a/Excel_Challenge_582 - Pivot on Min and Max_2.xlsx
+++ b/Excel_Challenge_582 - Pivot on Min and Max_2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C93ABF80-F683-4B54-AD18-CB3CF7F42472}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{016D9C75-0057-4074-9972-BA96EF54676D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{BB796D0A-1929-4DDD-A038-93396BD327EF}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{BB796D0A-1929-4DDD-A038-93396BD327EF}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
@@ -675,7 +675,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0027365-88D3-4720-A7D1-268188D0D3D1}">
   <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
@@ -1051,8 +1051,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F35A0C36-C234-477E-A992-B91BF6985A89}">
   <dimension ref="A1:X28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="V4" sqref="V4"/>
+    <sheetView topLeftCell="F10" workbookViewId="0">
+      <selection activeCell="V11" sqref="V11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1522,6 +1522,13 @@
       <c r="T11">
         <v>45355</v>
       </c>
+      <c r="V11" cm="1">
+        <f t="array" ref="V11:W13">_xlfn.XMATCH(_xlfn.UNIQUE(_xlfn.ANCHORARRAY(T4)),_xlfn.ANCHORARRAY( T4), , {1,-1})</f>
+        <v>1</v>
+      </c>
+      <c r="W11">
+        <v>6</v>
+      </c>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
@@ -1563,6 +1570,12 @@
       <c r="T12">
         <v>45355</v>
       </c>
+      <c r="V12">
+        <v>7</v>
+      </c>
+      <c r="W12">
+        <v>11</v>
+      </c>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
@@ -1603,6 +1616,12 @@
       </c>
       <c r="T13">
         <v>45355</v>
+      </c>
+      <c r="V13">
+        <v>12</v>
+      </c>
+      <c r="W13">
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.3">
@@ -2062,8 +2081,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F5F37A5-0EE7-458E-B4BC-B7722F86273D}">
   <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2520,8 +2539,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98D13AD8-E41C-4F96-8856-A1F4A1B18AE7}">
   <dimension ref="A1:Y26"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22:H26"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="S25" sqref="S25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>